<commit_message>
&& - 83454101 (1 часть) от 20.11.2025 https://meshok.net/
</commit_message>
<xml_diff>
--- a/Collections/EURO/Monaco/#EURO#Monaco#Commemorative#[2007-present]#UNC.xlsx
+++ b/Collections/EURO/Monaco/#EURO#Monaco#Commemorative#[2007-present]#UNC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lord_Alexator\Documents\CoinCollection\Collections\EURO\Monaco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC76BB22-62D0-4DDA-AF11-84525D60F569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166F2E2F-80F5-4A91-A17B-D4ECBB6981CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4170" yWindow="1430" windowWidth="33150" windowHeight="17560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2€" sheetId="1" r:id="rId1"/>
@@ -83,7 +83,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
   <si>
     <t>Year</t>
   </si>
@@ -560,7 +560,23 @@
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9BE5FF"/>
+          <bgColor rgb="FF9BE5FF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -655,9 +671,9 @@
     <filterColumn colId="2" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="1" dataCellStyle="Гиперссылка"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="№" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Link" dataDxfId="3" dataCellStyle="Гиперссылка"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description (single table, table set, mintage, prices):" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="1" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -932,7 +948,7 @@
       <pane xSplit="9" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1469,8 +1485,8 @@
       <c r="G19" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H19" s="24" t="s">
-        <v>4</v>
+      <c r="H19" s="28">
+        <v>1</v>
       </c>
       <c r="I19" s="11" t="str">
         <f t="shared" ref="I19:I21" si="6">IF(OR(AND(H19&gt;1,H19&lt;&gt;"-")),"Can exchange","")</f>
@@ -1525,8 +1541,8 @@
       <c r="G21" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="24" t="s">
-        <v>4</v>
+      <c r="H21" s="28">
+        <v>1</v>
       </c>
       <c r="I21" s="11" t="str">
         <f t="shared" si="6"/>
@@ -1569,12 +1585,12 @@
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="H7:H9">
-    <cfRule type="containsText" dxfId="10" priority="25" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="12" priority="29" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H7))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:H9">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1586,11 +1602,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
-    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
+    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="*-">
       <formula>NOT(ISERROR(SEARCH(("*-"),(H11))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H11">
+    <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H3">
+    <cfRule type="colorScale" priority="16">
+      <colorScale>
+        <cfvo type="formula" val="0"/>
+        <cfvo type="formula" val="1"/>
+        <cfvo type="formula" val="10"/>
+        <color rgb="FFFF9F9F"/>
+        <color rgb="FFD1E0B2"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H16 H18 H20 H22">
+    <cfRule type="containsText" dxfId="9" priority="13" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H12:H16 H18 H20 H22">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1602,13 +1652,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H3))))</formula>
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="containsText" dxfId="8" priority="19" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H4))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H3">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="H4:H6">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1619,12 +1669,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H16 H18 H20 H22">
+  <conditionalFormatting sqref="H17">
     <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H12))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H16 H18 H20 H22">
+  <conditionalFormatting sqref="H17">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1636,13 +1686,13 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H6">
-    <cfRule type="containsText" dxfId="6" priority="15" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H4))))</formula>
+  <conditionalFormatting sqref="H10">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:H6">
-    <cfRule type="colorScale" priority="16">
+  <conditionalFormatting sqref="H10">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="formula" val="0"/>
         <cfvo type="formula" val="1"/>
@@ -1653,29 +1703,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H17 H19">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H17))))</formula>
+  <conditionalFormatting sqref="H21">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H21))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H19 H17">
-    <cfRule type="colorScale" priority="6">
-      <colorScale>
-        <cfvo type="formula" val="0"/>
-        <cfvo type="formula" val="1"/>
-        <cfvo type="formula" val="10"/>
-        <color rgb="FFFF9F9F"/>
-        <color rgb="FFD1E0B2"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H10))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H10">
+  <conditionalFormatting sqref="H21">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="formula" val="0"/>
@@ -1687,12 +1720,12 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="*-">
-      <formula>NOT(ISERROR(SEARCH(("*-"),(H21))))</formula>
+  <conditionalFormatting sqref="H19">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="*-">
+      <formula>NOT(ISERROR(SEARCH(("*-"),(H19))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21">
+  <conditionalFormatting sqref="H19">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="formula" val="0"/>

</xml_diff>